<commit_message>
updated data dictionary with GCD tables
</commit_message>
<xml_diff>
--- a/cobra_db_data_dictionary.xlsx
+++ b/cobra_db_data_dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="22960" yWindow="2500" windowWidth="23960" windowHeight="25560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="391">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1068,6 +1068,246 @@
   </si>
   <si>
     <t>Internal records of form users and data entry</t>
+  </si>
+  <si>
+    <t>GCD Tables</t>
+  </si>
+  <si>
+    <t>gcd_issue</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>no_volume</t>
+  </si>
+  <si>
+    <t>display_volume_with_number</t>
+  </si>
+  <si>
+    <t>series_id</t>
+  </si>
+  <si>
+    <t>indicida_pub_not_printed</t>
+  </si>
+  <si>
+    <t>no_brand</t>
+  </si>
+  <si>
+    <t>publication_date</t>
+  </si>
+  <si>
+    <t>key_date</t>
+  </si>
+  <si>
+    <t>sort_code</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>page_count</t>
+  </si>
+  <si>
+    <t>page_count_uncertain</t>
+  </si>
+  <si>
+    <t>indicia_frequency</t>
+  </si>
+  <si>
+    <t>editing</t>
+  </si>
+  <si>
+    <t>no_editing</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>is_indexed</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>valid_isbn</t>
+  </si>
+  <si>
+    <t>no_isbn</t>
+  </si>
+  <si>
+    <t>variant_of_id</t>
+  </si>
+  <si>
+    <t>variant_name</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>Unique ID for each issue record</t>
+  </si>
+  <si>
+    <t>Volume that issue was published within</t>
+  </si>
+  <si>
+    <t>ID from associated series</t>
+  </si>
+  <si>
+    <t>Publication date of issue</t>
+  </si>
+  <si>
+    <t>gcd_series</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sort_name</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>year_began</t>
+  </si>
+  <si>
+    <t>year_began_uncertain</t>
+  </si>
+  <si>
+    <t>year_ended</t>
+  </si>
+  <si>
+    <t>year_ended_uncertain</t>
+  </si>
+  <si>
+    <t>publication_dates</t>
+  </si>
+  <si>
+    <t>is_current</t>
+  </si>
+  <si>
+    <t>publisher_id</t>
+  </si>
+  <si>
+    <t>country_id</t>
+  </si>
+  <si>
+    <t>tracking_notes</t>
+  </si>
+  <si>
+    <t>publication_notes</t>
+  </si>
+  <si>
+    <t>has_gallery</t>
+  </si>
+  <si>
+    <t>open_reserve</t>
+  </si>
+  <si>
+    <t>issue_count</t>
+  </si>
+  <si>
+    <t>has_indicia_frequency</t>
+  </si>
+  <si>
+    <t>has_isbn</t>
+  </si>
+  <si>
+    <t>has_barcode</t>
+  </si>
+  <si>
+    <t>has_issue_title</t>
+  </si>
+  <si>
+    <t>has_volume</t>
+  </si>
+  <si>
+    <t>is_comics_publication</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>dimensions</t>
+  </si>
+  <si>
+    <t>Unique ID for each series record</t>
+  </si>
+  <si>
+    <t>Series title</t>
+  </si>
+  <si>
+    <t>Publication date range of series (unreliable)</t>
+  </si>
+  <si>
+    <t>ID from associated publisher</t>
+  </si>
+  <si>
+    <t>ID from associated country of publication</t>
+  </si>
+  <si>
+    <t>gcd_publisher</t>
+  </si>
+  <si>
+    <t>gcd_country</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>is_master</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>imprint_count</t>
+  </si>
+  <si>
+    <t>brand_count</t>
+  </si>
+  <si>
+    <t>indicia_publisher_count</t>
+  </si>
+  <si>
+    <t>series_count</t>
+  </si>
+  <si>
+    <t>Name of publisher</t>
+  </si>
+  <si>
+    <t>Unique ID for each publisher record</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Unique ID for each country record</t>
+  </si>
+  <si>
+    <t>Two letter country code</t>
+  </si>
+  <si>
+    <t>Name of country</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1376,8 +1616,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1397,8 +1646,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1490,8 +1751,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1501,6 +1765,12 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1510,6 +1780,12 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1837,16 +2113,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A92" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="1" bestFit="1" customWidth="1"/>
@@ -3508,7 +3784,7 @@
     </row>
     <row r="110" spans="1:6" ht="16">
       <c r="A110" s="30" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B110" s="30"/>
       <c r="C110" s="30"/>
@@ -3518,17 +3794,15 @@
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="13" t="s">
-        <v>279</v>
+        <v>312</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>280</v>
+        <v>313</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>261</v>
-      </c>
+        <v>342</v>
+      </c>
+      <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
         <v>210</v>
       </c>
@@ -3537,194 +3811,1107 @@
     <row r="112" spans="1:6">
       <c r="A112" s="14"/>
       <c r="B112" s="6" t="s">
-        <v>281</v>
+        <v>314</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>261</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D112" s="6"/>
       <c r="E112" s="6"/>
       <c r="F112" s="7"/>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" s="14"/>
       <c r="B113" s="17" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D113" s="17" t="s">
-        <v>261</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="D113" s="17"/>
       <c r="E113" s="17"/>
       <c r="F113" s="18"/>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="14"/>
       <c r="B114" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="D114" s="17" t="s">
-        <v>261</v>
-      </c>
+        <v>316</v>
+      </c>
+      <c r="C114" s="6"/>
+      <c r="D114" s="17"/>
       <c r="E114" s="17"/>
       <c r="F114" s="18"/>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="14"/>
-      <c r="B115" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="E115" s="8"/>
-      <c r="F115" s="9"/>
+      <c r="B115" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="C115" s="6"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="18"/>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="D116" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="E116" s="4"/>
-      <c r="F116" s="5"/>
+      <c r="A116" s="14"/>
+      <c r="B116" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="F116" s="18" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="14"/>
-      <c r="B117" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="E117" s="8"/>
-      <c r="F117" s="9"/>
+      <c r="B117" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C117" s="6"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="18"/>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F118" s="5"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="C118" s="6"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="18"/>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="14"/>
-      <c r="B119" s="6" t="s">
-        <v>290</v>
+      <c r="B119" s="17" t="s">
+        <v>321</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E119" s="6"/>
-      <c r="F119" s="7"/>
-    </row>
-    <row r="120" spans="1:6" ht="24">
+        <v>345</v>
+      </c>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="18"/>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" s="14"/>
-      <c r="B120" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E120" s="6"/>
-      <c r="F120" s="7"/>
+      <c r="B120" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="C120" s="6"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="18"/>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="14"/>
-      <c r="B121" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E121" s="6"/>
-      <c r="F121" s="7"/>
+      <c r="B121" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="18"/>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="14"/>
-      <c r="B122" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D122" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E122" s="6"/>
-      <c r="F122" s="7"/>
+      <c r="B122" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C122" s="6"/>
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="18"/>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="14"/>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="18"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="14"/>
+      <c r="B124" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C124" s="6"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="18"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="14"/>
+      <c r="B125" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="C125" s="6"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="18"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="14"/>
+      <c r="B126" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="C126" s="6"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="18"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="14"/>
+      <c r="B127" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="C127" s="6"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="18"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="14"/>
+      <c r="B128" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C128" s="6"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="18"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="14"/>
+      <c r="B129" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C129" s="6"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="18"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="14"/>
+      <c r="B130" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C130" s="6"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="18"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="14"/>
+      <c r="B131" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C131" s="6"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="18"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="14"/>
+      <c r="B132" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="C132" s="6"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="18"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="14"/>
+      <c r="B133" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="C133" s="6"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="18"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="14"/>
+      <c r="B134" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="C134" s="6"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="18"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="14"/>
+      <c r="B135" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C135" s="6"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="18"/>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="14"/>
+      <c r="B136" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="C136" s="6"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="18"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="14"/>
+      <c r="B137" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C137" s="6"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="18"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="14"/>
+      <c r="B138" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C138" s="6"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="18"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="14"/>
+      <c r="B139" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C139" s="6"/>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
+      <c r="F139" s="9"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D140" s="4"/>
+      <c r="E140" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="14"/>
+      <c r="B141" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+      <c r="F141" s="7"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="14"/>
+      <c r="B142" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="C142" s="6"/>
+      <c r="D142" s="17"/>
+      <c r="E142" s="17"/>
+      <c r="F142" s="18"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="14"/>
+      <c r="B143" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="C143" s="6"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="17"/>
+      <c r="F143" s="18"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="14"/>
+      <c r="B144" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="C144" s="6"/>
+      <c r="D144" s="17"/>
+      <c r="E144" s="17"/>
+      <c r="F144" s="18"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="14"/>
+      <c r="B145" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="C145" s="6"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="17"/>
+      <c r="F145" s="18"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="14"/>
+      <c r="B146" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C146" s="6"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+      <c r="F146" s="18"/>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="14"/>
+      <c r="B147" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C147" s="6"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
+      <c r="F147" s="18"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="14"/>
+      <c r="B148" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="18"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="14"/>
+      <c r="B149" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C149" s="6"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="18"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="14"/>
+      <c r="B150" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="F150" s="18" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="14"/>
+      <c r="B151" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D151" s="17"/>
+      <c r="E151" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="F151" s="18" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="14"/>
+      <c r="B152" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="C152" s="6"/>
+      <c r="D152" s="17"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="18"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="14"/>
+      <c r="B153" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C153" s="6"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="18"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="14"/>
+      <c r="B154" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="C154" s="6"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="18"/>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="14"/>
+      <c r="B155" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="C155" s="6"/>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17"/>
+      <c r="F155" s="18"/>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="14"/>
+      <c r="B156" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="C156" s="6"/>
+      <c r="D156" s="17"/>
+      <c r="E156" s="17"/>
+      <c r="F156" s="18"/>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="14"/>
+      <c r="B157" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C157" s="6"/>
+      <c r="D157" s="17"/>
+      <c r="E157" s="17"/>
+      <c r="F157" s="18"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="14"/>
+      <c r="B158" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C158" s="6"/>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17"/>
+      <c r="F158" s="18"/>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="14"/>
+      <c r="B159" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C159" s="6"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17"/>
+      <c r="F159" s="18"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="14"/>
+      <c r="B160" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C160" s="6"/>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17"/>
+      <c r="F160" s="18"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="14"/>
+      <c r="B161" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="C161" s="6"/>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17"/>
+      <c r="F161" s="18"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="14"/>
+      <c r="B162" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C162" s="6"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="18"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="14"/>
+      <c r="B163" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C163" s="6"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="18"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="14"/>
+      <c r="B164" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="C164" s="6"/>
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="18"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="14"/>
+      <c r="B165" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="C165" s="6"/>
+      <c r="D165" s="17"/>
+      <c r="E165" s="17"/>
+      <c r="F165" s="18"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="14"/>
+      <c r="B166" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="C166" s="6"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="18"/>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="14"/>
+      <c r="B167" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C167" s="6"/>
+      <c r="D167" s="17"/>
+      <c r="E167" s="17"/>
+      <c r="F167" s="18"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="14"/>
+      <c r="B168" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="C168" s="6"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="18"/>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="14"/>
+      <c r="B169" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="C169" s="6"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="8"/>
+      <c r="F169" s="9"/>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="D170" s="4"/>
+      <c r="E170" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F170" s="5"/>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="14"/>
+      <c r="B171" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="7"/>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="14"/>
+      <c r="B172" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D172" s="17"/>
+      <c r="E172" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="F172" s="18" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="14"/>
+      <c r="B173" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="C173" s="6"/>
+      <c r="D173" s="17"/>
+      <c r="E173" s="17"/>
+      <c r="F173" s="18"/>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="14"/>
+      <c r="B174" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C174" s="6"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="18"/>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="14"/>
+      <c r="B175" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C175" s="6"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="18"/>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="14"/>
+      <c r="B176" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C176" s="6"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="18"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="14"/>
+      <c r="B177" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="C177" s="6"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="18"/>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="14"/>
+      <c r="B178" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="C178" s="6"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="18"/>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="14"/>
+      <c r="B179" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C179" s="6"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="18"/>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="14"/>
+      <c r="B180" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="C180" s="6"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="18"/>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="14"/>
+      <c r="B181" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="C181" s="6"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="18"/>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="14"/>
+      <c r="B182" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="C182" s="6"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="18"/>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="14"/>
+      <c r="B183" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C183" s="6"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="18"/>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="14"/>
+      <c r="B184" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="C184" s="6"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="18"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="14"/>
+      <c r="B185" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C185" s="6"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="18"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="14"/>
+      <c r="B186" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C186" s="6"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="18"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="14"/>
+      <c r="B187" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="C187" s="6"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="18"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="14"/>
+      <c r="B188" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="C188" s="6"/>
+      <c r="D188" s="17"/>
+      <c r="E188" s="17"/>
+      <c r="F188" s="18"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="14"/>
+      <c r="B189" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C189" s="6"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="8"/>
+      <c r="F189" s="9"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E190" s="4"/>
+      <c r="F190" s="5"/>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="14"/>
+      <c r="B191" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="C191" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="D191" s="23"/>
+      <c r="E191" s="23"/>
+      <c r="F191" s="31"/>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="14"/>
+      <c r="B192" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D192" s="8"/>
+      <c r="E192" s="8"/>
+      <c r="F192" s="9"/>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="24"/>
+      <c r="B193" s="24"/>
+      <c r="C193" s="24"/>
+      <c r="D193" s="24"/>
+      <c r="E193" s="24"/>
+      <c r="F193" s="24"/>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="23"/>
+      <c r="B194" s="23"/>
+      <c r="C194" s="23"/>
+      <c r="D194" s="23"/>
+      <c r="E194" s="23"/>
+      <c r="F194" s="23"/>
+    </row>
+    <row r="195" spans="1:6" ht="16">
+      <c r="A195" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="B195" s="30"/>
+      <c r="C195" s="30"/>
+      <c r="D195" s="30"/>
+      <c r="E195" s="30"/>
+      <c r="F195" s="30"/>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F196" s="5"/>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="14"/>
+      <c r="B197" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D197" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E197" s="6"/>
+      <c r="F197" s="7"/>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="14"/>
+      <c r="B198" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D198" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E198" s="17"/>
+      <c r="F198" s="18"/>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="14"/>
+      <c r="B199" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D199" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E199" s="17"/>
+      <c r="F199" s="18"/>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="14"/>
+      <c r="B200" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D200" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E200" s="8"/>
+      <c r="F200" s="9"/>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E201" s="4"/>
+      <c r="F201" s="5"/>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="14"/>
+      <c r="B202" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C202" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D202" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="E202" s="8"/>
+      <c r="F202" s="9"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E203" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F203" s="5"/>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="14"/>
+      <c r="B204" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C204" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D204" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E204" s="6"/>
+      <c r="F204" s="7"/>
+    </row>
+    <row r="205" spans="1:6" ht="24">
+      <c r="A205" s="14"/>
+      <c r="B205" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C205" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D205" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E205" s="6"/>
+      <c r="F205" s="7"/>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="14"/>
+      <c r="B206" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E206" s="6"/>
+      <c r="F206" s="7"/>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" s="14"/>
+      <c r="B207" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C207" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D207" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E207" s="6"/>
+      <c r="F207" s="7"/>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" s="14"/>
+      <c r="B208" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C208" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="D123" s="6" t="s">
+      <c r="D208" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E123" s="6"/>
-      <c r="F123" s="7"/>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="15"/>
-      <c r="B124" s="8" t="s">
+      <c r="E208" s="6"/>
+      <c r="F208" s="7"/>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" s="15"/>
+      <c r="B209" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C124" s="8" t="s">
+      <c r="C209" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D124" s="8" t="s">
+      <c r="D209" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E124" s="8"/>
-      <c r="F124" s="9"/>
+      <c r="E209" s="8"/>
+      <c r="F209" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A195:F195"/>
     <mergeCell ref="A110:F110"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>